<commit_message>
change to jason's timesheet
</commit_message>
<xml_diff>
--- a/Time sheet/MCI-Timetsheet(Jason-week-2).xlsx
+++ b/Time sheet/MCI-Timetsheet(Jason-week-2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/MCI_2021/MCI Project/Week 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/MCI_2021/MCI_Project/Team-024/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D692324-F5C5-6F44-81BC-FFEBB4BA3613}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A48A67-A65E-AB48-854E-35D9BD05F8C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="500" windowWidth="19320" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="500" windowWidth="19320" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +761,7 @@
         <v>0.625</v>
       </c>
       <c r="E6" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>19</v>
@@ -819,6 +819,12 @@
         <v>13</v>
       </c>
       <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
@@ -873,7 +879,7 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="12">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>22</v>
@@ -938,7 +944,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E9" s="12">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>24</v>
@@ -1103,7 +1109,7 @@
       </c>
       <c r="E12" s="8">
         <f>SUM(E6:E11)</f>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1118,7 +1124,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C8:D11 C6:D6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>